<commit_message>
Austria market Power calculation excel sheet update added
</commit_message>
<xml_diff>
--- a/Test Data/Power_Calculation_Default_Values.xlsx
+++ b/Test Data/Power_Calculation_Default_Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB78C23-A7DF-4197-8237-9AF20ADFD47A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57900254-30D9-4752-9FE0-DAC3560B0FF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="106">
   <si>
     <t>Color Codes</t>
   </si>
@@ -530,6 +530,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -539,7 +540,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,13 +848,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1209,7 +1209,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1230,13 +1230,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1611,13 +1611,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1971,7 +1971,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1996,13 +1996,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2036,7 +2036,7 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="7"/>
@@ -2212,7 +2212,9 @@
       <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>51</v>
       </c>
@@ -2282,7 +2284,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>63</v>
@@ -2356,7 +2358,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2381,13 +2383,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2420,7 +2422,7 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>102</v>
       </c>
       <c r="C4" s="7"/>
@@ -2596,7 +2598,9 @@
       <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>51</v>
       </c>
@@ -2666,7 +2670,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>63</v>
@@ -2740,7 +2744,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2765,13 +2769,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -2805,7 +2809,7 @@
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>104</v>
       </c>
       <c r="C4" s="7"/>
@@ -2981,7 +2985,9 @@
       <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="E9" s="14" t="s">
         <v>51</v>
       </c>
@@ -3051,7 +3057,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>63</v>
@@ -3150,13 +3156,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3535,13 +3541,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3920,13 +3926,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4312,13 +4318,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4702,13 +4708,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -4991,7 +4997,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:W10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5016,13 +5022,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5376,7 +5382,7 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5388,13 +5394,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5758,13 +5764,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>